<commit_message>
started excel comparison per class to udnerstand performance difference between test50 and 1996 abstracts; introduced knew test50 with random_state 2, must rename new file (P6)
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts.xlsx
+++ b/models/evaluations/evaluation_prompts.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9E03BF-1B46-4841-875C-A6A26F1DD533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C20EC1-4C1A-2845-BAA1-9C80F3B4B76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="21380" windowHeight="14060" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="21380" windowHeight="14060" activeTab="1" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation_Summary" sheetId="3" r:id="rId1"/>
-    <sheet name="notes&amp;acronyms" sheetId="2" r:id="rId2"/>
-    <sheet name="other layout (incomplete)" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="notes&amp;acronyms" sheetId="2" r:id="rId3"/>
+    <sheet name="other layout (incomplete)" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="90">
   <si>
     <t>prompt description</t>
   </si>
@@ -310,12 +311,81 @@
   <si>
     <t>example for significant performance differences on test50 vs. 1996 abstracts =&gt; Shirin will try to find a reason for this till the meeting</t>
   </si>
+  <si>
+    <t>support</t>
+  </si>
+  <si>
+    <t>Prompt ID</t>
+  </si>
+  <si>
+    <t>Human-systematic-review</t>
+  </si>
+  <si>
+    <t>Human-RCT-drug-intervention</t>
+  </si>
+  <si>
+    <t>Human-RCT-non-drug-intervention</t>
+  </si>
+  <si>
+    <t>Human-RCT-non-intervention</t>
+  </si>
+  <si>
+    <t>Human-case-report</t>
+  </si>
+  <si>
+    <t>Human-non-RCT-drug-intervention</t>
+  </si>
+  <si>
+    <t>Human-non-RCT-non-drug-intervention</t>
+  </si>
+  <si>
+    <t>Animal-systematic-review</t>
+  </si>
+  <si>
+    <t>Animal-drug-intervention</t>
+  </si>
+  <si>
+    <t>Animal-non-drug-intervention</t>
+  </si>
+  <si>
+    <t>Animal-other</t>
+  </si>
+  <si>
+    <t>Non-systematic-review</t>
+  </si>
+  <si>
+    <t>In-vitro-study</t>
+  </si>
+  <si>
+    <t>Clinical-study-protocol</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>micro avg</t>
+  </si>
+  <si>
+    <t>macro avg</t>
+  </si>
+  <si>
+    <t>weighted avg</t>
+  </si>
+  <si>
+    <t>gpt-3.5 1996</t>
+  </si>
+  <si>
+    <t>gpt-3.5 test50</t>
+  </si>
+  <si>
+    <t>gpt-3.5 test50 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -347,6 +417,14 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -421,7 +499,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -444,6 +522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,7 +864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
   <dimension ref="B2:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+    <sheetView zoomScale="67" workbookViewId="0">
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
@@ -1710,6 +1789,1181 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE0D96C-177E-5749-9148-C444A4078D5A}">
+  <dimension ref="A1:V19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>67</v>
+      </c>
+      <c r="O1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1">
+        <v>0.5</v>
+      </c>
+      <c r="S1">
+        <v>0.5</v>
+      </c>
+      <c r="T1">
+        <v>0.5</v>
+      </c>
+      <c r="U1">
+        <v>2</v>
+      </c>
+      <c r="V1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2">
+        <v>0.53763440860214995</v>
+      </c>
+      <c r="L2">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="M2">
+        <v>0.65359477124182996</v>
+      </c>
+      <c r="N2">
+        <v>60</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3">
+        <v>0.452380952380952</v>
+      </c>
+      <c r="L3">
+        <v>0.82608695652173902</v>
+      </c>
+      <c r="M3">
+        <v>0.58461538461538398</v>
+      </c>
+      <c r="N3">
+        <v>23</v>
+      </c>
+      <c r="O3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K4">
+        <v>0.63888888888888795</v>
+      </c>
+      <c r="L4">
+        <v>0.60526315789473595</v>
+      </c>
+      <c r="M4">
+        <v>0.62162162162162105</v>
+      </c>
+      <c r="N4">
+        <v>38</v>
+      </c>
+      <c r="O4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="R5">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="S5">
+        <v>0.75</v>
+      </c>
+      <c r="T5">
+        <v>0.461538</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6">
+        <v>0.4</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.57142857142857095</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6">
+        <v>23</v>
+      </c>
+      <c r="J6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6">
+        <v>0.312883435582822</v>
+      </c>
+      <c r="L6">
+        <v>0.88695652173912998</v>
+      </c>
+      <c r="M6">
+        <v>0.46258503401360501</v>
+      </c>
+      <c r="N6">
+        <v>115</v>
+      </c>
+      <c r="O6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6">
+        <v>0.5</v>
+      </c>
+      <c r="S6">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="T6">
+        <v>0.4</v>
+      </c>
+      <c r="U6">
+        <v>3</v>
+      </c>
+      <c r="V6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="D7">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7">
+        <v>24</v>
+      </c>
+      <c r="J7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7">
+        <v>0.60227272727272696</v>
+      </c>
+      <c r="L7">
+        <v>0.41085271317829403</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.488479262672811</v>
+      </c>
+      <c r="N7">
+        <v>129</v>
+      </c>
+      <c r="O7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="R7">
+        <v>0.13333300000000001</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0.235294</v>
+      </c>
+      <c r="U7">
+        <v>2</v>
+      </c>
+      <c r="V7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <v>0.27272727272727199</v>
+      </c>
+      <c r="D8">
+        <v>0.75</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.39999999999999902</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8">
+        <v>25</v>
+      </c>
+      <c r="J8" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8">
+        <v>0.23140495867768501</v>
+      </c>
+      <c r="L8">
+        <v>0.53846153846153799</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.32369942196531698</v>
+      </c>
+      <c r="N8">
+        <v>156</v>
+      </c>
+      <c r="O8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9">
+        <v>26</v>
+      </c>
+      <c r="J9" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10">
+        <v>27</v>
+      </c>
+      <c r="J10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10">
+        <v>0.57857142857142796</v>
+      </c>
+      <c r="L10">
+        <v>0.83505154639175205</v>
+      </c>
+      <c r="M10">
+        <v>0.683544303797468</v>
+      </c>
+      <c r="N10">
+        <v>97</v>
+      </c>
+      <c r="O10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>2</v>
+      </c>
+      <c r="V10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11">
+        <v>28</v>
+      </c>
+      <c r="J11" t="s">
+        <v>78</v>
+      </c>
+      <c r="K11">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="L11">
+        <v>0.51851851851851805</v>
+      </c>
+      <c r="M11">
+        <v>0.54901960784313697</v>
+      </c>
+      <c r="N11">
+        <v>27</v>
+      </c>
+      <c r="O11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q11" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="R11">
+        <v>0.25</v>
+      </c>
+      <c r="S11">
+        <v>0.5</v>
+      </c>
+      <c r="T11">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="U11">
+        <v>2</v>
+      </c>
+      <c r="V11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="E12">
+        <v>0.8</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12">
+        <v>29</v>
+      </c>
+      <c r="J12" t="s">
+        <v>79</v>
+      </c>
+      <c r="K12">
+        <v>0.51020408163265296</v>
+      </c>
+      <c r="L12">
+        <v>0.476190476190476</v>
+      </c>
+      <c r="M12">
+        <v>0.49261083743842299</v>
+      </c>
+      <c r="N12">
+        <v>105</v>
+      </c>
+      <c r="O12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>0.3</v>
+      </c>
+      <c r="T12">
+        <v>0.461538</v>
+      </c>
+      <c r="U12">
+        <v>10</v>
+      </c>
+      <c r="V12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>0.14285714285714199</v>
+      </c>
+      <c r="E13">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K13">
+        <v>0.621848739495798</v>
+      </c>
+      <c r="L13">
+        <v>0.23052959501557599</v>
+      </c>
+      <c r="M13">
+        <v>0.33636363636363598</v>
+      </c>
+      <c r="N13">
+        <v>321</v>
+      </c>
+      <c r="O13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q13" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="T13">
+        <v>0.5</v>
+      </c>
+      <c r="U13">
+        <v>3</v>
+      </c>
+      <c r="V13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14">
+        <v>31</v>
+      </c>
+      <c r="J14" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="L14">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="M14">
+        <v>0.3</v>
+      </c>
+      <c r="N14">
+        <v>54</v>
+      </c>
+      <c r="O14" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15">
+        <v>32</v>
+      </c>
+      <c r="J15" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0.375</v>
+      </c>
+      <c r="M15">
+        <v>0.54545454545454497</v>
+      </c>
+      <c r="N15">
+        <v>8</v>
+      </c>
+      <c r="O15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="R15">
+        <v>0.72727299999999995</v>
+      </c>
+      <c r="S15">
+        <v>0.36363600000000001</v>
+      </c>
+      <c r="T15">
+        <v>0.484848</v>
+      </c>
+      <c r="U15">
+        <v>22</v>
+      </c>
+      <c r="V15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.81818181818181801</v>
+      </c>
+      <c r="D16">
+        <v>0.45</v>
+      </c>
+      <c r="E16">
+        <v>0.58064516129032195</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16">
+        <v>33</v>
+      </c>
+      <c r="J16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.68998410174880698</v>
+      </c>
+      <c r="L16">
+        <v>0.50582750582750502</v>
+      </c>
+      <c r="M16">
+        <v>0.58372562205783396</v>
+      </c>
+      <c r="N16">
+        <v>858</v>
+      </c>
+      <c r="O16" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="R16">
+        <v>0.44</v>
+      </c>
+      <c r="S16">
+        <v>0.44</v>
+      </c>
+      <c r="T16">
+        <v>0.44</v>
+      </c>
+      <c r="U16">
+        <v>50</v>
+      </c>
+      <c r="V16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17">
+        <v>0.6</v>
+      </c>
+      <c r="D17">
+        <v>0.6</v>
+      </c>
+      <c r="E17">
+        <v>0.6</v>
+      </c>
+      <c r="F17">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17">
+        <v>34</v>
+      </c>
+      <c r="J17" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17">
+        <v>0.50050100200400804</v>
+      </c>
+      <c r="L17">
+        <v>0.50075187969924795</v>
+      </c>
+      <c r="M17">
+        <v>0.50062640942119696</v>
+      </c>
+      <c r="N17">
+        <v>1995</v>
+      </c>
+      <c r="O17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="R17">
+        <v>0.362929</v>
+      </c>
+      <c r="S17">
+        <v>0.33868700000000002</v>
+      </c>
+      <c r="T17">
+        <v>0.29176999999999997</v>
+      </c>
+      <c r="U17">
+        <v>50</v>
+      </c>
+      <c r="V17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18">
+        <v>0.45812409812409799</v>
+      </c>
+      <c r="D18">
+        <v>0.51174603174603095</v>
+      </c>
+      <c r="E18">
+        <v>0.44939750810718498</v>
+      </c>
+      <c r="F18">
+        <v>50</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18">
+        <v>35</v>
+      </c>
+      <c r="J18" t="s">
+        <v>85</v>
+      </c>
+      <c r="K18">
+        <v>0.48139636784838002</v>
+      </c>
+      <c r="L18">
+        <v>0.48428627235298799</v>
+      </c>
+      <c r="M18">
+        <v>0.441687603272374</v>
+      </c>
+      <c r="N18">
+        <v>1995</v>
+      </c>
+      <c r="O18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="S18">
+        <v>0.44</v>
+      </c>
+      <c r="T18" s="3">
+        <v>0.47930899999999999</v>
+      </c>
+      <c r="U18">
+        <v>50</v>
+      </c>
+      <c r="V18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.71651948051948</v>
+      </c>
+      <c r="D19">
+        <v>0.6</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.60289298515104905</v>
+      </c>
+      <c r="F19">
+        <v>50</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19">
+        <v>36</v>
+      </c>
+      <c r="J19" t="s">
+        <v>86</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.58481217714644396</v>
+      </c>
+      <c r="L19">
+        <v>0.50075187969924795</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.50386771305181499</v>
+      </c>
+      <c r="N19">
+        <v>1995</v>
+      </c>
+      <c r="O19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7C6A26-482D-C04F-982C-E2185B2D0E99}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -1778,7 +3032,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90BC467B-3818-CB45-90D9-07E8BC875ED8}">
   <dimension ref="A1:L66"/>
   <sheetViews>

</xml_diff>

<commit_message>
did experiments with P6 while I changed random_state to see if performance changes and to try to explain differences in performance test50 vs 1996
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts.xlsx
+++ b/models/evaluations/evaluation_prompts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C20EC1-4C1A-2845-BAA1-9C80F3B4B76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8279F537-4A86-124B-9C16-1A0A386313DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="500" windowWidth="21380" windowHeight="14060" activeTab="1" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="92">
   <si>
     <t>prompt description</t>
   </si>
@@ -379,6 +379,12 @@
   </si>
   <si>
     <t>gpt-3.5 test50 2</t>
+  </si>
+  <si>
+    <t>gpt-3.5 test50_random_state3</t>
+  </si>
+  <si>
+    <t>gpt-3.5 test50_random_state4</t>
   </si>
 </sst>
 </file>
@@ -427,7 +433,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -455,6 +461,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -523,6 +535,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1790,10 +1803,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE0D96C-177E-5749-9148-C444A4078D5A}">
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="67" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1841,23 +1854,17 @@
       <c r="P1" t="s">
         <v>89</v>
       </c>
-      <c r="Q1" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="R1">
-        <v>0.5</v>
-      </c>
-      <c r="S1">
-        <v>0.5</v>
-      </c>
-      <c r="T1">
-        <v>0.5</v>
-      </c>
-      <c r="U1">
+      <c r="R1" t="s">
         <v>2</v>
       </c>
-      <c r="V1" t="s">
-        <v>15</v>
+      <c r="S1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -1903,20 +1910,20 @@
       <c r="O2" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="16" t="s">
-        <v>70</v>
+      <c r="Q2" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>0.33333299999999999</v>
       </c>
       <c r="S2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V2" t="s">
         <v>15</v>
@@ -1965,8 +1972,8 @@
       <c r="O3" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="16" t="s">
-        <v>71</v>
+      <c r="Q3" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -2027,8 +2034,8 @@
       <c r="O4" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="16" t="s">
-        <v>72</v>
+      <c r="Q4" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -2089,20 +2096,20 @@
       <c r="O5" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="16" t="s">
-        <v>73</v>
+      <c r="Q5" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="R5">
-        <v>0.33333299999999999</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>0.461538</v>
+        <v>0</v>
       </c>
       <c r="U5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V5" t="s">
         <v>15</v>
@@ -2151,20 +2158,20 @@
       <c r="O6" t="s">
         <v>15</v>
       </c>
-      <c r="Q6" s="16" t="s">
-        <v>74</v>
+      <c r="Q6" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="R6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S6">
-        <v>0.33333299999999999</v>
+        <v>1</v>
       </c>
       <c r="T6">
-        <v>0.4</v>
+        <v>0.57142899999999996</v>
       </c>
       <c r="U6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V6" t="s">
         <v>15</v>
@@ -2213,20 +2220,20 @@
       <c r="O7" t="s">
         <v>15</v>
       </c>
-      <c r="Q7" s="16" t="s">
-        <v>75</v>
+      <c r="Q7" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="R7">
-        <v>0.13333300000000001</v>
+        <v>0.5</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>0.33333299999999999</v>
       </c>
       <c r="T7">
-        <v>0.235294</v>
+        <v>0.4</v>
       </c>
       <c r="U7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V7" t="s">
         <v>15</v>
@@ -2275,20 +2282,20 @@
       <c r="O8" t="s">
         <v>15</v>
       </c>
-      <c r="Q8" s="16" t="s">
-        <v>76</v>
+      <c r="Q8" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>0.16666700000000001</v>
       </c>
       <c r="S8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>0.28571400000000002</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V8" t="s">
         <v>15</v>
@@ -2337,8 +2344,8 @@
       <c r="O9" t="s">
         <v>15</v>
       </c>
-      <c r="Q9" s="16" t="s">
-        <v>77</v>
+      <c r="Q9" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -2399,20 +2406,20 @@
       <c r="O10" t="s">
         <v>15</v>
       </c>
-      <c r="Q10" s="16" t="s">
-        <v>78</v>
+      <c r="Q10" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V10" t="s">
         <v>15</v>
@@ -2461,17 +2468,17 @@
       <c r="O11" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="16" t="s">
-        <v>79</v>
+      <c r="Q11" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="R11">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="S11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="T11">
-        <v>0.33333299999999999</v>
+        <v>1</v>
       </c>
       <c r="U11">
         <v>2</v>
@@ -2523,20 +2530,20 @@
       <c r="O12" t="s">
         <v>15</v>
       </c>
-      <c r="Q12" s="16" t="s">
-        <v>80</v>
+      <c r="Q12" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="R12">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="S12">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="T12">
-        <v>0.461538</v>
+        <v>0.33333299999999999</v>
       </c>
       <c r="U12">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="V12" t="s">
         <v>15</v>
@@ -2585,20 +2592,20 @@
       <c r="O13" t="s">
         <v>15</v>
       </c>
-      <c r="Q13" s="16" t="s">
-        <v>81</v>
+      <c r="Q13" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="R13">
         <v>1</v>
       </c>
       <c r="S13">
-        <v>0.33333299999999999</v>
+        <v>0.3</v>
       </c>
       <c r="T13">
-        <v>0.5</v>
+        <v>0.461538</v>
       </c>
       <c r="U13">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="V13" t="s">
         <v>15</v>
@@ -2647,20 +2654,20 @@
       <c r="O14" t="s">
         <v>15</v>
       </c>
-      <c r="Q14" s="16" t="s">
-        <v>82</v>
+      <c r="Q14" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>0.33333299999999999</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V14" t="s">
         <v>15</v>
@@ -2709,20 +2716,20 @@
       <c r="O15" t="s">
         <v>15</v>
       </c>
-      <c r="Q15" s="16" t="s">
-        <v>83</v>
+      <c r="Q15" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="R15">
-        <v>0.72727299999999995</v>
+        <v>0</v>
       </c>
       <c r="S15">
-        <v>0.36363600000000001</v>
+        <v>0</v>
       </c>
       <c r="T15">
-        <v>0.484848</v>
+        <v>0</v>
       </c>
       <c r="U15">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="V15" t="s">
         <v>15</v>
@@ -2771,20 +2778,20 @@
       <c r="O16" t="s">
         <v>15</v>
       </c>
-      <c r="Q16" s="16" t="s">
-        <v>84</v>
+      <c r="Q16" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="R16">
-        <v>0.44</v>
+        <v>0.90909099999999998</v>
       </c>
       <c r="S16">
-        <v>0.44</v>
+        <v>0.45454499999999998</v>
       </c>
       <c r="T16">
-        <v>0.44</v>
+        <v>0.60606099999999996</v>
       </c>
       <c r="U16">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="V16" t="s">
         <v>15</v>
@@ -2833,17 +2840,17 @@
       <c r="O17" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" s="16" t="s">
-        <v>85</v>
+      <c r="Q17" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="R17">
-        <v>0.362929</v>
+        <v>0.5</v>
       </c>
       <c r="S17">
-        <v>0.33868700000000002</v>
+        <v>0.5</v>
       </c>
       <c r="T17">
-        <v>0.29176999999999997</v>
+        <v>0.5</v>
       </c>
       <c r="U17">
         <v>50</v>
@@ -2895,17 +2902,17 @@
       <c r="O18" t="s">
         <v>15</v>
       </c>
-      <c r="Q18" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="R18" s="3">
-        <v>0.71199999999999997</v>
+      <c r="Q18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="R18">
+        <v>0.33727299999999999</v>
       </c>
       <c r="S18">
-        <v>0.44</v>
-      </c>
-      <c r="T18" s="3">
-        <v>0.47930899999999999</v>
+        <v>0.36141400000000001</v>
+      </c>
+      <c r="T18">
+        <v>0.297205</v>
       </c>
       <c r="U18">
         <v>50</v>
@@ -2942,19 +2949,756 @@
       <c r="J19" t="s">
         <v>86</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="17">
         <v>0.58481217714644396</v>
       </c>
       <c r="L19">
         <v>0.50075187969924795</v>
       </c>
-      <c r="M19" s="3">
+      <c r="M19" s="17">
         <v>0.50386771305181499</v>
       </c>
       <c r="N19">
         <v>1995</v>
       </c>
       <c r="O19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="R19" s="3">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="S19">
+        <v>0.5</v>
+      </c>
+      <c r="T19" s="17">
+        <v>0.53345100000000001</v>
+      </c>
+      <c r="U19">
+        <v>50</v>
+      </c>
+      <c r="V19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" t="s">
+        <v>91</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="O21" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22">
+        <v>0.5</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0.5</v>
+      </c>
+      <c r="E24">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26">
+        <v>0.125</v>
+      </c>
+      <c r="D26">
+        <v>0.5</v>
+      </c>
+      <c r="E26">
+        <v>0.2</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="K26">
+        <v>0.44444400000000001</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26">
+        <v>0.61538499999999996</v>
+      </c>
+      <c r="N26">
+        <v>4</v>
+      </c>
+      <c r="O26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27">
+        <v>0.75</v>
+      </c>
+      <c r="D27">
+        <v>0.75</v>
+      </c>
+      <c r="E27">
+        <v>0.75</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J27" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="K27">
+        <v>0.33333299999999999</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>0.5</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28">
+        <v>0.57142899999999996</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>0.72727299999999995</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="J28" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K28">
+        <v>0.222222</v>
+      </c>
+      <c r="L28">
+        <v>0.5</v>
+      </c>
+      <c r="M28">
+        <v>0.30769200000000002</v>
+      </c>
+      <c r="N28">
+        <v>4</v>
+      </c>
+      <c r="O28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>0</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>2</v>
+      </c>
+      <c r="O30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+      <c r="E31">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0.75</v>
+      </c>
+      <c r="E32">
+        <v>0.85714299999999999</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>0.5</v>
+      </c>
+      <c r="M32">
+        <v>0.66666700000000001</v>
+      </c>
+      <c r="N32">
+        <v>4</v>
+      </c>
+      <c r="O32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33">
+        <v>0.6</v>
+      </c>
+      <c r="D33">
+        <v>0.375</v>
+      </c>
+      <c r="E33">
+        <v>0.461538</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+      <c r="G33" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="K33">
+        <v>0.75</v>
+      </c>
+      <c r="L33">
+        <v>0.3</v>
+      </c>
+      <c r="M33">
+        <v>0.42857099999999998</v>
+      </c>
+      <c r="N33">
+        <v>10</v>
+      </c>
+      <c r="O33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36">
+        <v>0.85714299999999999</v>
+      </c>
+      <c r="D36">
+        <v>0.57142899999999996</v>
+      </c>
+      <c r="E36">
+        <v>0.68571400000000005</v>
+      </c>
+      <c r="F36">
+        <v>21</v>
+      </c>
+      <c r="G36" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="K36">
+        <v>0.6875</v>
+      </c>
+      <c r="L36">
+        <v>0.52381</v>
+      </c>
+      <c r="M36">
+        <v>0.59459499999999998</v>
+      </c>
+      <c r="N36">
+        <v>21</v>
+      </c>
+      <c r="O36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37">
+        <v>0.62</v>
+      </c>
+      <c r="D37">
+        <v>0.62</v>
+      </c>
+      <c r="E37">
+        <v>0.62</v>
+      </c>
+      <c r="F37">
+        <v>50</v>
+      </c>
+      <c r="G37" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="K37">
+        <v>0.54</v>
+      </c>
+      <c r="L37">
+        <v>0.54</v>
+      </c>
+      <c r="M37">
+        <v>0.54</v>
+      </c>
+      <c r="N37">
+        <v>50</v>
+      </c>
+      <c r="O37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38">
+        <v>0.46023799999999998</v>
+      </c>
+      <c r="D38">
+        <v>0.46309499999999998</v>
+      </c>
+      <c r="E38">
+        <v>0.42322199999999999</v>
+      </c>
+      <c r="F38">
+        <v>50</v>
+      </c>
+      <c r="G38" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="K38">
+        <v>0.32916699999999999</v>
+      </c>
+      <c r="L38">
+        <v>0.38825399999999999</v>
+      </c>
+      <c r="M38">
+        <v>0.31863799999999998</v>
+      </c>
+      <c r="N38">
+        <v>50</v>
+      </c>
+      <c r="O38" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B39" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39">
+        <v>0.756714</v>
+      </c>
+      <c r="D39">
+        <v>0.62</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.64993299999999998</v>
+      </c>
+      <c r="F39">
+        <v>50</v>
+      </c>
+      <c r="G39" t="s">
+        <v>15</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="K39">
+        <v>0.63875000000000004</v>
+      </c>
+      <c r="L39">
+        <v>0.54</v>
+      </c>
+      <c r="M39">
+        <v>0.53929000000000005</v>
+      </c>
+      <c r="N39">
+        <v>50</v>
+      </c>
+      <c r="O39" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tried labelin first half, second half to go, P9_1, added prompting strategies P11_5 and P12
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts.xlsx
+++ b/models/evaluations/evaluation_prompts.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8279F537-4A86-124B-9C16-1A0A386313DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B81643-B6BA-364C-88F8-B5B52DD89AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="21380" windowHeight="14060" activeTab="1" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="21380" windowHeight="14060" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation_Summary" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="playing with random_state" sheetId="4" r:id="rId2"/>
     <sheet name="notes&amp;acronyms" sheetId="2" r:id="rId3"/>
     <sheet name="other layout (incomplete)" sheetId="1" r:id="rId4"/>
   </sheets>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="105">
   <si>
     <t>prompt description</t>
   </si>
@@ -220,9 +220,6 @@
     </r>
   </si>
   <si>
-    <t>&lt;=&gt; control per class</t>
-  </si>
-  <si>
     <t>CC: shortened annotation guidelines, only table; added separate mention of labels; reduced mentions of  what classification should apply to, format and where those infos occur</t>
   </si>
   <si>
@@ -386,12 +383,54 @@
   <si>
     <t>gpt-3.5 test50_random_state4</t>
   </si>
+  <si>
+    <t>P11_5</t>
+  </si>
+  <si>
+    <t>no protocol in sample -&gt; didn't test</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: based upon P11 (CoT placement with best results) but with shortened annotation guidelines</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: shortened annotation guidelines, only table &amp;Let's think step by step (CoT)</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: shortened annotation guidelines, only table &amp;Let's think step by step (CoT) put in different place than P11</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: shortened annotation guidelines, only table &amp;Let's think step by step (CoT) put in different place than P11 and P11_1</t>
+  </si>
+  <si>
+    <t>summary gpt-3.5 first half of abstracts</t>
+  </si>
+  <si>
+    <t>summary gpt-3.5 second half of abstracts</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P9_1</t>
+  </si>
+  <si>
+    <t>description of P11- P11_2 was wrong (only table!); P9_1 new, P11_5 and P12 new; first half and then second half new</t>
+  </si>
+  <si>
+    <t>CoT&amp;CC: short explanation why label was chosen (wording of P7) + shortened annotation guidelines, only table</t>
+  </si>
+  <si>
+    <t>2CoT&amp;CC: P11 &amp; explanation (CoT) based on P9</t>
+  </si>
+  <si>
+    <t>does P9/P9_1 really give explanation????</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -428,6 +467,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -511,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -536,6 +581,8 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
-  <dimension ref="B2:Y25"/>
+  <dimension ref="B2:AI32"/>
   <sheetViews>
-    <sheetView zoomScale="67" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="J2" zoomScale="76" workbookViewId="0">
+      <selection activeCell="AF27" sqref="AF27:AF28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -891,9 +938,11 @@
     <col min="16" max="16" width="1.83203125" customWidth="1"/>
     <col min="20" max="20" width="2" customWidth="1"/>
     <col min="22" max="22" width="1.83203125" customWidth="1"/>
+    <col min="26" max="26" width="2.6640625" customWidth="1"/>
+    <col min="31" max="31" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:35" x14ac:dyDescent="0.2">
       <c r="E2" s="13" t="s">
         <v>19</v>
       </c>
@@ -918,8 +967,18 @@
       </c>
       <c r="X2" s="13"/>
       <c r="Y2" s="13"/>
-    </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AB2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AG2" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AH2" s="13"/>
+      <c r="AI2" s="13"/>
+    </row>
+    <row r="3" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -973,13 +1032,37 @@
       <c r="Y3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4">
         <v>0.53082051282051201</v>
@@ -1021,13 +1104,19 @@
       <c r="Y4" s="2">
         <v>0.40595713</v>
       </c>
-    </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E5">
         <v>0.61448717948717901</v>
@@ -1069,13 +1158,19 @@
       <c r="Y5" s="2">
         <v>0.33070487999999998</v>
       </c>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2">
         <v>0.19866666999999999</v>
@@ -1099,13 +1194,19 @@
       <c r="U6" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF6" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7">
         <v>0.3</v>
@@ -1128,13 +1229,19 @@
       <c r="U7" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF7" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="2">
         <v>0.55655677999999997</v>
@@ -1174,13 +1281,19 @@
       <c r="U8" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF8" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E9" s="2">
         <v>0.54193650999999998</v>
@@ -1220,13 +1333,19 @@
       <c r="U9" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF9" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="2">
         <v>0.56226496000000004</v>
@@ -1266,13 +1385,19 @@
       <c r="U10" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF10" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="2">
         <v>0.54122221999999998</v>
@@ -1302,8 +1427,14 @@
       <c r="U11" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1331,13 +1462,19 @@
       <c r="U12" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF12" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="2">
         <v>0.45187878999999997</v>
@@ -1377,13 +1514,22 @@
       <c r="U13" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF13" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>13</v>
@@ -1403,8 +1549,14 @@
       <c r="U14" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF14" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1439,8 +1591,14 @@
       <c r="U15" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="AA15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF15" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:35" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
@@ -1475,13 +1633,31 @@
       <c r="U16" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="AA16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB16">
+        <v>0.57588099999999998</v>
+      </c>
+      <c r="AC16">
+        <v>0.49398799999999998</v>
+      </c>
+      <c r="AD16">
+        <v>0.49834000000000001</v>
+      </c>
+      <c r="AF16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG16" s="17"/>
+      <c r="AH16" s="17"/>
+      <c r="AI16" s="17"/>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17">
         <v>0.58333333333333304</v>
@@ -1510,13 +1686,19 @@
       <c r="U17" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="AA17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF17" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18">
         <v>0.41599999999999998</v>
@@ -1539,13 +1721,19 @@
       <c r="U18" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="AA18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF18" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19">
         <v>0.58186813186813102</v>
@@ -1574,229 +1762,371 @@
       <c r="U19" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="AA19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF19" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E20">
+        <v>0.50682499999999997</v>
+      </c>
+      <c r="F20">
+        <v>0.36</v>
+      </c>
+      <c r="G20">
+        <v>0.34594900000000001</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="O20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="U20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA20" s="8"/>
+      <c r="AF20" s="8"/>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C21" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>0.655555555555555</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>0.38</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>0.40454545454545399</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K21" s="2">
         <v>0.51212380999999996</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L21" s="2">
         <v>0.27669173000000002</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M21" s="2">
         <v>0.24118174000000001</v>
       </c>
-      <c r="O20" s="8" t="s">
+      <c r="O21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="U20" s="8" t="s">
+      <c r="U21" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
+      <c r="AA21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF21" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21">
+      <c r="C22" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22">
         <v>0.60133333333333305</v>
       </c>
-      <c r="F21">
+      <c r="F22">
         <v>0.46</v>
       </c>
-      <c r="G21">
+      <c r="G22">
         <v>0.44543589743589701</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K21" s="2">
+      <c r="K22" s="2">
         <v>0.49125333999999998</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L22" s="2">
         <v>0.30476189999999997</v>
       </c>
-      <c r="M21" s="2">
+      <c r="M22" s="2">
         <v>0.28231458999999998</v>
       </c>
-      <c r="O21" s="8" t="s">
+      <c r="O22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="U21" s="8" t="s">
+      <c r="U22" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B22" s="8" t="s">
+      <c r="AA22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF22" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22">
+      <c r="C23" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23">
         <v>0.54952380952380897</v>
       </c>
-      <c r="F22">
+      <c r="F23">
         <v>0.36</v>
       </c>
-      <c r="G22">
+      <c r="G23">
         <v>0.32374703557312201</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K23" s="2">
         <v>0.48442905000000003</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L23" s="2">
         <v>0.31578947000000002</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M23" s="2">
         <v>0.29657749999999999</v>
       </c>
-      <c r="O22" s="8" t="s">
+      <c r="O23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="U22" s="8" t="s">
+      <c r="U23" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B23" s="8" t="s">
+      <c r="AA23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF23" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23">
+      <c r="C24" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24">
         <v>0.47060606060605997</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <v>0.42</v>
       </c>
-      <c r="G23">
+      <c r="G24">
         <v>0.38861538461538397</v>
       </c>
-      <c r="I23" s="8" t="s">
+      <c r="I24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K24" s="2">
         <v>0.58530731000000003</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L24" s="2">
         <v>0.32130325999999998</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M24" s="2">
         <v>0.31364184000000001</v>
       </c>
-      <c r="O23" s="8" t="s">
+      <c r="O24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="U23" s="8" t="s">
+      <c r="U24" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B24" s="8" t="s">
+      <c r="AA24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF24" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C25" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <v>0.69446154000000004</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F25" s="2">
         <v>0.52</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G25" s="2">
         <v>0.53914439000000003</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K24">
-        <v>0.60768</v>
-      </c>
-      <c r="L24">
-        <v>0.43959900000000002</v>
-      </c>
-      <c r="M24">
-        <v>0.435585</v>
-      </c>
-      <c r="N24" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="O24" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="U24" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B25" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0.57015583999999997</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0.54</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0.51797541999999996</v>
       </c>
       <c r="H25" s="2"/>
       <c r="I25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25">
+        <v>0.60768</v>
+      </c>
+      <c r="L25">
+        <v>0.43959900000000002</v>
+      </c>
+      <c r="M25">
+        <v>0.435585</v>
+      </c>
+      <c r="N25" s="5"/>
+      <c r="O25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF25" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K25" s="2">
+      <c r="C26" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.57015583999999997</v>
+      </c>
+      <c r="F26" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0.51797541999999996</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K26" s="2">
         <v>0.58421833999999995</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L26" s="2">
         <v>0.47518797000000002</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M26" s="2">
         <v>0.48158585999999998</v>
       </c>
-      <c r="O25" s="8" t="s">
+      <c r="O26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="U25" s="8" t="s">
+      <c r="U26" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="AA26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF26" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="I27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="O27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="U27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF27" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B28" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="I28" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="O28" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="U28" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA28" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF28" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="C30" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>101</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="AG2:AI2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="W2:Y2"/>
     <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="AB2:AD2"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1805,8 +2135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE0D96C-177E-5749-9148-C444A4078D5A}">
   <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="67" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:J21"/>
+    <sheetView topLeftCell="B7" zoomScale="50" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1816,7 +2146,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1828,13 +2158,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
         <v>67</v>
       </c>
-      <c r="G1" t="s">
-        <v>68</v>
-      </c>
       <c r="I1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K1" t="s">
         <v>2</v>
@@ -1846,13 +2176,13 @@
         <v>4</v>
       </c>
       <c r="N1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" t="s">
         <v>67</v>
       </c>
-      <c r="O1" t="s">
-        <v>68</v>
-      </c>
       <c r="P1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R1" t="s">
         <v>2</v>
@@ -1864,7 +2194,7 @@
         <v>4</v>
       </c>
       <c r="U1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
@@ -1872,7 +2202,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1893,7 +2223,7 @@
         <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K2">
         <v>0.53763440860214995</v>
@@ -1911,7 +2241,7 @@
         <v>15</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="R2">
         <v>0.33333299999999999</v>
@@ -1934,7 +2264,7 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
@@ -1955,7 +2285,7 @@
         <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K3">
         <v>0.452380952380952</v>
@@ -1973,7 +2303,7 @@
         <v>15</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -1996,7 +2326,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -2017,7 +2347,7 @@
         <v>21</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K4">
         <v>0.63888888888888795</v>
@@ -2035,7 +2365,7 @@
         <v>15</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="R4">
         <v>0</v>
@@ -2058,7 +2388,7 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2079,7 +2409,7 @@
         <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -2097,7 +2427,7 @@
         <v>15</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R5">
         <v>0</v>
@@ -2120,7 +2450,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6">
         <v>0.4</v>
@@ -2141,7 +2471,7 @@
         <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K6">
         <v>0.312883435582822</v>
@@ -2159,7 +2489,7 @@
         <v>15</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R6">
         <v>0.4</v>
@@ -2182,7 +2512,7 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7">
         <v>0.66666666666666596</v>
@@ -2203,7 +2533,7 @@
         <v>24</v>
       </c>
       <c r="J7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K7">
         <v>0.60227272727272696</v>
@@ -2221,7 +2551,7 @@
         <v>15</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R7">
         <v>0.5</v>
@@ -2244,7 +2574,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8">
         <v>0.27272727272727199</v>
@@ -2265,7 +2595,7 @@
         <v>25</v>
       </c>
       <c r="J8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K8">
         <v>0.23140495867768501</v>
@@ -2283,7 +2613,7 @@
         <v>15</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R8">
         <v>0.16666700000000001</v>
@@ -2306,7 +2636,7 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2327,7 +2657,7 @@
         <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -2345,7 +2675,7 @@
         <v>15</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -2368,7 +2698,7 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10">
         <v>0.71428571428571397</v>
@@ -2389,7 +2719,7 @@
         <v>27</v>
       </c>
       <c r="J10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K10">
         <v>0.57857142857142796</v>
@@ -2407,7 +2737,7 @@
         <v>15</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -2430,7 +2760,7 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -2451,7 +2781,7 @@
         <v>28</v>
       </c>
       <c r="J11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K11">
         <v>0.58333333333333304</v>
@@ -2469,7 +2799,7 @@
         <v>15</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R11">
         <v>1</v>
@@ -2492,7 +2822,7 @@
         <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -2513,7 +2843,7 @@
         <v>29</v>
       </c>
       <c r="J12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K12">
         <v>0.51020408163265296</v>
@@ -2531,7 +2861,7 @@
         <v>15</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R12">
         <v>0.25</v>
@@ -2554,7 +2884,7 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13">
         <v>0.5</v>
@@ -2575,7 +2905,7 @@
         <v>30</v>
       </c>
       <c r="J13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K13">
         <v>0.621848739495798</v>
@@ -2593,7 +2923,7 @@
         <v>15</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R13">
         <v>1</v>
@@ -2616,7 +2946,7 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14">
         <v>0.5</v>
@@ -2637,7 +2967,7 @@
         <v>31</v>
       </c>
       <c r="J14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K14">
         <v>0.46153846153846101</v>
@@ -2655,7 +2985,7 @@
         <v>15</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R14">
         <v>0.5</v>
@@ -2678,7 +3008,7 @@
         <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -2699,7 +3029,7 @@
         <v>32</v>
       </c>
       <c r="J15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -2717,7 +3047,7 @@
         <v>15</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R15">
         <v>0</v>
@@ -2740,7 +3070,7 @@
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="3">
         <v>0.81818181818181801</v>
@@ -2761,7 +3091,7 @@
         <v>33</v>
       </c>
       <c r="J16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K16" s="3">
         <v>0.68998410174880698</v>
@@ -2779,7 +3109,7 @@
         <v>15</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R16">
         <v>0.90909099999999998</v>
@@ -2802,7 +3132,7 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17">
         <v>0.6</v>
@@ -2823,7 +3153,7 @@
         <v>34</v>
       </c>
       <c r="J17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K17">
         <v>0.50050100200400804</v>
@@ -2841,7 +3171,7 @@
         <v>15</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R17">
         <v>0.5</v>
@@ -2864,7 +3194,7 @@
         <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18">
         <v>0.45812409812409799</v>
@@ -2885,7 +3215,7 @@
         <v>35</v>
       </c>
       <c r="J18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K18">
         <v>0.48139636784838002</v>
@@ -2903,7 +3233,7 @@
         <v>15</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R18">
         <v>0.33727299999999999</v>
@@ -2926,7 +3256,7 @@
         <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="3">
         <v>0.71651948051948</v>
@@ -2947,7 +3277,7 @@
         <v>36</v>
       </c>
       <c r="J19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K19" s="17">
         <v>0.58481217714644396</v>
@@ -2965,7 +3295,7 @@
         <v>15</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R19" s="3">
         <v>0.76200000000000001</v>
@@ -2985,7 +3315,7 @@
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" t="s">
         <v>2</v>
@@ -2997,10 +3327,10 @@
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K21" s="16" t="s">
         <v>2</v>
@@ -3012,15 +3342,15 @@
         <v>4</v>
       </c>
       <c r="N21" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="O21" s="16" t="s">
         <v>67</v>
-      </c>
-      <c r="O21" s="16" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22">
         <v>0.5</v>
@@ -3038,7 +3368,7 @@
         <v>15</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K22">
         <v>0.5</v>
@@ -3058,7 +3388,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -3076,7 +3406,7 @@
         <v>15</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -3096,7 +3426,7 @@
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3114,7 +3444,7 @@
         <v>15</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -3134,7 +3464,7 @@
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3152,7 +3482,7 @@
         <v>15</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -3172,7 +3502,7 @@
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26">
         <v>0.125</v>
@@ -3190,7 +3520,7 @@
         <v>15</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K26">
         <v>0.44444400000000001</v>
@@ -3210,7 +3540,7 @@
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27">
         <v>0.75</v>
@@ -3228,7 +3558,7 @@
         <v>15</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K27">
         <v>0.33333299999999999</v>
@@ -3248,7 +3578,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28">
         <v>0.57142899999999996</v>
@@ -3266,7 +3596,7 @@
         <v>15</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K28">
         <v>0.222222</v>
@@ -3286,7 +3616,7 @@
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -3304,7 +3634,7 @@
         <v>15</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -3324,7 +3654,7 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30">
         <v>0.5</v>
@@ -3342,7 +3672,7 @@
         <v>15</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -3362,7 +3692,7 @@
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3380,7 +3710,7 @@
         <v>15</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -3400,7 +3730,7 @@
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3418,7 +3748,7 @@
         <v>15</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -3438,7 +3768,7 @@
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C33">
         <v>0.6</v>
@@ -3456,7 +3786,7 @@
         <v>15</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K33">
         <v>0.75</v>
@@ -3476,7 +3806,7 @@
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -3494,7 +3824,7 @@
         <v>15</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -3514,7 +3844,7 @@
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -3532,7 +3862,7 @@
         <v>15</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -3552,7 +3882,7 @@
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C36">
         <v>0.85714299999999999</v>
@@ -3570,7 +3900,7 @@
         <v>15</v>
       </c>
       <c r="J36" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K36">
         <v>0.6875</v>
@@ -3590,7 +3920,7 @@
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C37">
         <v>0.62</v>
@@ -3608,7 +3938,7 @@
         <v>15</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K37">
         <v>0.54</v>
@@ -3628,7 +3958,7 @@
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C38">
         <v>0.46023799999999998</v>
@@ -3646,7 +3976,7 @@
         <v>15</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K38">
         <v>0.32916699999999999</v>
@@ -3666,7 +3996,7 @@
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C39">
         <v>0.756714</v>
@@ -3684,7 +4014,7 @@
         <v>15</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K39">
         <v>0.63875000000000004</v>
@@ -3735,13 +4065,13 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
P12, P11_5, P6 secondhalf
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts.xlsx
+++ b/models/evaluations/evaluation_prompts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B81643-B6BA-364C-88F8-B5B52DD89AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51948F83-EF1E-FE45-907C-37FB8D223CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="500" windowWidth="21380" windowHeight="14060" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -924,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
   <dimension ref="B2:AI32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" zoomScale="76" workbookViewId="0">
-      <selection activeCell="AF27" sqref="AF27:AF28"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2056,15 +2056,27 @@
       <c r="C27" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
+      <c r="E27">
+        <v>0.52248499999999998</v>
+      </c>
+      <c r="F27">
+        <v>0.46</v>
+      </c>
+      <c r="G27">
+        <v>0.44462800000000002</v>
+      </c>
       <c r="I27" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
+      <c r="K27">
+        <v>0.54705800000000004</v>
+      </c>
+      <c r="L27">
+        <v>0.34536299999999998</v>
+      </c>
+      <c r="M27">
+        <v>0.33741700000000002</v>
+      </c>
       <c r="O27" s="8" t="s">
         <v>91</v>
       </c>
@@ -2085,15 +2097,27 @@
       <c r="C28" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
+      <c r="E28">
+        <v>0.61444399999999999</v>
+      </c>
+      <c r="F28">
+        <v>0.4</v>
+      </c>
+      <c r="G28">
+        <v>0.38377099999999997</v>
+      </c>
       <c r="I28" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
+      <c r="K28">
+        <v>0.564828</v>
+      </c>
+      <c r="L28">
+        <v>0.27468700000000001</v>
+      </c>
+      <c r="M28">
+        <v>0.24404999999999999</v>
+      </c>
       <c r="O28" s="8" t="s">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
started new experiments with test-dataset (0.2test) P1, P2, P3_1
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts.xlsx
+++ b/models/evaluations/evaluation_prompts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30082865-E6B5-1445-9059-A178CE3713A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8CE6A4-2525-E448-928B-F1E147D2BE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluation_Summary" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="108">
   <si>
     <t>prompt description</t>
   </si>
@@ -424,6 +424,15 @@
   </si>
   <si>
     <t>description of P11- P11_2 was wrong (only table!); P9_1 new, P11_5 and P12 new; first half and then second half P6 new</t>
+  </si>
+  <si>
+    <t>summary 0.2test gpt-3.5</t>
+  </si>
+  <si>
+    <t>summary 0.2test gpt-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -587,6 +596,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,8 +605,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -935,63 +944,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
-  <dimension ref="B2:AI32"/>
+  <dimension ref="B2:AU32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="114" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="69" customWidth="1"/>
+    <col min="3" max="3" width="68.6640625" customWidth="1"/>
     <col min="4" max="4" width="2.83203125" customWidth="1"/>
     <col min="8" max="8" width="1.83203125" customWidth="1"/>
     <col min="10" max="10" width="2.5" customWidth="1"/>
-    <col min="14" max="14" width="6.83203125" customWidth="1"/>
-    <col min="16" max="16" width="1.83203125" customWidth="1"/>
-    <col min="20" max="20" width="2" customWidth="1"/>
-    <col min="22" max="22" width="1.83203125" customWidth="1"/>
-    <col min="26" max="26" width="2.6640625" customWidth="1"/>
-    <col min="31" max="31" width="2.1640625" customWidth="1"/>
+    <col min="14" max="14" width="2.6640625" customWidth="1"/>
+    <col min="16" max="16" width="3.1640625" customWidth="1"/>
+    <col min="18" max="18" width="11.5" customWidth="1"/>
+    <col min="20" max="20" width="2.6640625" customWidth="1"/>
+    <col min="22" max="22" width="2" customWidth="1"/>
+    <col min="24" max="24" width="13" customWidth="1"/>
+    <col min="26" max="26" width="2" customWidth="1"/>
+    <col min="28" max="28" width="2.6640625" customWidth="1"/>
+    <col min="32" max="32" width="2" customWidth="1"/>
+    <col min="33" max="33" width="10" customWidth="1"/>
+    <col min="34" max="34" width="2.33203125" customWidth="1"/>
+    <col min="38" max="38" width="2" customWidth="1"/>
+    <col min="43" max="43" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:35" x14ac:dyDescent="0.2">
-      <c r="E2" s="16" t="s">
+    <row r="2" spans="2:47" x14ac:dyDescent="0.2">
+      <c r="E2" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="K2" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="Q2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="K2" s="16" t="s">
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="6"/>
+      <c r="W2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="Q2" s="16" t="s">
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
+      <c r="AC2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="W2" s="16" t="s">
+      <c r="AD2" s="18"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AI2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="AB2" s="16" t="s">
+      <c r="AJ2" s="18"/>
+      <c r="AK2" s="18"/>
+      <c r="AN2" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AG2" s="16" t="s">
+      <c r="AO2" s="18"/>
+      <c r="AP2" s="18"/>
+      <c r="AS2" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="AH2" s="16"/>
-      <c r="AI2" s="16"/>
-    </row>
-    <row r="3" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AT2" s="18"/>
+      <c r="AU2" s="18"/>
+    </row>
+    <row r="3" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1007,7 +1034,6 @@
       <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="1"/>
       <c r="I3" s="7" t="s">
         <v>1</v>
       </c>
@@ -1048,29 +1074,54 @@
       <c r="AA3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AF3" s="7" t="s">
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AK3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AR3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1078,54 +1129,69 @@
         <v>59</v>
       </c>
       <c r="E4">
-        <v>0.53082051282051201</v>
+        <v>0.469831</v>
       </c>
       <c r="F4">
-        <v>0.36</v>
+        <v>0.25742599999999999</v>
       </c>
       <c r="G4">
-        <v>0.34943196672608401</v>
+        <v>0.210198</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="2">
-        <v>0.50564805999999995</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0.25513784</v>
-      </c>
-      <c r="M4" s="2">
-        <v>0.20566124999999999</v>
-      </c>
       <c r="O4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
+      <c r="Q4">
+        <v>0.53082051282051201</v>
+      </c>
+      <c r="R4">
+        <v>0.36</v>
+      </c>
+      <c r="S4">
+        <v>0.34943196672608401</v>
+      </c>
       <c r="U4" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="V4" s="17"/>
       <c r="W4" s="2">
-        <v>0.59366505000000003</v>
+        <v>0.50564805999999995</v>
       </c>
       <c r="X4" s="2">
-        <v>0.42506265999999998</v>
+        <v>0.25513784</v>
       </c>
       <c r="Y4" s="2">
-        <v>0.40595713</v>
+        <v>0.20566124999999999</v>
       </c>
       <c r="AA4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AI4" s="2">
+        <v>0.59366505000000003</v>
+      </c>
+      <c r="AJ4" s="2">
+        <v>0.42506265999999998</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>0.40595713</v>
+      </c>
+      <c r="AM4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR4" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
@@ -1133,1048 +1199,1275 @@
         <v>60</v>
       </c>
       <c r="E5">
-        <v>0.61448717948717901</v>
+        <v>0.65417800000000004</v>
       </c>
       <c r="F5">
-        <v>0.28000000000000003</v>
+        <v>0.225248</v>
       </c>
       <c r="G5">
-        <v>0.28206060606060601</v>
+        <v>0.17084299999999999</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="2">
-        <v>0.52365876</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0.21804510999999999</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0.16039635999999999</v>
-      </c>
       <c r="O5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
+      <c r="Q5">
+        <v>0.61448717948717901</v>
+      </c>
+      <c r="R5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="S5">
+        <v>0.28206060606060601</v>
+      </c>
       <c r="U5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="W5" s="2">
-        <v>0.54637108999999995</v>
+        <v>0.52365876</v>
       </c>
       <c r="X5" s="2">
-        <v>0.36791980000000002</v>
+        <v>0.21804510999999999</v>
       </c>
       <c r="Y5" s="2">
-        <v>0.33070487999999998</v>
+        <v>0.16039635999999999</v>
       </c>
       <c r="AA5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="AF5" s="8" t="s">
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AI5" s="2">
+        <v>0.54637108999999995</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>0.36791980000000002</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>0.33070487999999998</v>
+      </c>
+      <c r="AM5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="AR5" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="2">
-        <v>0.19866666999999999</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0.20141176</v>
-      </c>
-      <c r="H6" s="2"/>
+      <c r="D6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
       <c r="I6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
       <c r="O6" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="Q6" s="2">
+        <v>0.19866666999999999</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0.24</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.20141176</v>
+      </c>
+      <c r="T6" s="2"/>
       <c r="U6" s="9" t="s">
         <v>20</v>
       </c>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+      <c r="Y6" s="12"/>
       <c r="AA6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AF6" s="9" t="s">
+      <c r="AG6" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AR6" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E7">
-        <v>0.3</v>
-      </c>
-      <c r="F7">
-        <v>0.06</v>
-      </c>
-      <c r="G7">
-        <v>9.9999999999999895E-2</v>
-      </c>
+      <c r="D7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
       <c r="I7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
       <c r="O7" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="Q7">
+        <v>0.3</v>
+      </c>
+      <c r="R7">
+        <v>0.06</v>
+      </c>
+      <c r="S7">
+        <v>9.9999999999999895E-2</v>
+      </c>
       <c r="U7" s="9" t="s">
         <v>7</v>
       </c>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
       <c r="AA7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AF7" s="9" t="s">
+      <c r="AG7" s="9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="AR7" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="2">
-        <v>0.55655677999999997</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.42</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0.38225550000000003</v>
-      </c>
-      <c r="H8" s="2"/>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8">
+        <v>0.59226599999999996</v>
+      </c>
+      <c r="F8">
+        <v>0.31930700000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.29668600000000001</v>
+      </c>
       <c r="I8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="2">
-        <v>0.57991552999999996</v>
-      </c>
-      <c r="L8" s="2">
-        <v>0.30175438999999998</v>
-      </c>
-      <c r="M8" s="2">
-        <v>0.27339846000000001</v>
-      </c>
       <c r="O8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="Q8" s="2">
-        <v>0.73085714000000002</v>
+        <v>0.55655677999999997</v>
       </c>
       <c r="R8" s="2">
-        <v>0.64</v>
+        <v>0.42</v>
       </c>
       <c r="S8" s="2">
-        <v>0.66312265999999997</v>
+        <v>0.38225550000000003</v>
       </c>
       <c r="T8" s="2"/>
       <c r="U8" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="W8" s="2">
+        <v>0.57991552999999996</v>
+      </c>
+      <c r="X8" s="2">
+        <v>0.30175438999999998</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>0.27339846000000001</v>
+      </c>
       <c r="AA8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AF8" s="8" t="s">
+      <c r="AC8" s="2">
+        <v>0.73085714000000002</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="AE8" s="2">
+        <v>0.66312265999999997</v>
+      </c>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR8" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="2">
-        <v>0.54193650999999998</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.42</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.41297931999999998</v>
-      </c>
-      <c r="H9" s="2"/>
+      <c r="D9" t="s">
+        <v>107</v>
+      </c>
       <c r="I9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="2">
-        <v>0.48737355999999998</v>
-      </c>
-      <c r="L9" s="2">
-        <v>0.31578947000000002</v>
-      </c>
-      <c r="M9" s="2">
-        <v>0.29975924999999998</v>
-      </c>
       <c r="O9" s="8" t="s">
         <v>9</v>
       </c>
       <c r="Q9" s="2">
-        <v>0.72961905000000005</v>
+        <v>0.54193650999999998</v>
       </c>
       <c r="R9" s="2">
-        <v>0.6</v>
+        <v>0.42</v>
       </c>
       <c r="S9" s="2">
-        <v>0.63242423999999997</v>
+        <v>0.41297931999999998</v>
       </c>
       <c r="T9" s="2"/>
       <c r="U9" s="8" t="s">
         <v>9</v>
       </c>
+      <c r="W9" s="2">
+        <v>0.48737355999999998</v>
+      </c>
+      <c r="X9" s="2">
+        <v>0.31578947000000002</v>
+      </c>
+      <c r="Y9" s="2">
+        <v>0.29975924999999998</v>
+      </c>
       <c r="AA9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="AF9" s="8" t="s">
+      <c r="AC9" s="2">
+        <v>0.72961905000000005</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>0.63242423999999997</v>
+      </c>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AR9" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="2">
-        <v>0.56226496000000004</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.34</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0.34794871999999999</v>
-      </c>
-      <c r="H10" s="2"/>
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
       <c r="I10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="2">
-        <v>0.48597420000000002</v>
-      </c>
-      <c r="L10" s="2">
-        <v>0.28671679</v>
-      </c>
-      <c r="M10" s="2">
-        <v>0.25912464000000002</v>
-      </c>
       <c r="O10" s="8" t="s">
         <v>10</v>
       </c>
       <c r="Q10" s="2">
-        <v>0.66476190000000002</v>
+        <v>0.56226496000000004</v>
       </c>
       <c r="R10" s="2">
-        <v>0.38</v>
+        <v>0.34</v>
       </c>
       <c r="S10" s="2">
-        <v>0.46771021000000002</v>
+        <v>0.34794871999999999</v>
       </c>
       <c r="T10" s="2"/>
       <c r="U10" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="W10" s="2">
+        <v>0.48597420000000002</v>
+      </c>
+      <c r="X10" s="2">
+        <v>0.28671679</v>
+      </c>
+      <c r="Y10" s="2">
+        <v>0.25912464000000002</v>
+      </c>
       <c r="AA10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="AF10" s="8" t="s">
+      <c r="AC10" s="2">
+        <v>0.66476190000000002</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>0.46771021000000002</v>
+      </c>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR10" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="2">
-        <v>0.54122221999999998</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.38</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.35797403</v>
-      </c>
-      <c r="H11" s="2"/>
+      <c r="D11" t="s">
+        <v>107</v>
+      </c>
       <c r="I11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="2">
-        <v>0.51644239000000003</v>
-      </c>
-      <c r="L11" s="2">
-        <v>0.31528822000000001</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0.30435465</v>
-      </c>
       <c r="O11" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="Q11" s="2">
+        <v>0.54122221999999998</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0.35797403</v>
+      </c>
+      <c r="T11" s="2"/>
       <c r="U11" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="W11" s="2">
+        <v>0.51644239000000003</v>
+      </c>
+      <c r="X11" s="2">
+        <v>0.31528822000000001</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>0.30435465</v>
+      </c>
       <c r="AA11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AF11" s="8" t="s">
+      <c r="AG11" s="8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AR11" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="E12">
-        <v>0.266666666666666</v>
-      </c>
-      <c r="F12">
-        <v>0.08</v>
-      </c>
-      <c r="G12">
-        <v>0.123076923076923</v>
-      </c>
+      <c r="D12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
       <c r="I12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
       <c r="O12" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="Q12">
+        <v>0.266666666666666</v>
+      </c>
+      <c r="R12">
+        <v>0.08</v>
+      </c>
+      <c r="S12">
+        <v>0.123076923076923</v>
+      </c>
       <c r="U12" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="W12" s="12"/>
+      <c r="X12" s="12"/>
+      <c r="Y12" s="12"/>
       <c r="AA12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AF12" s="9" t="s">
+      <c r="AG12" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR12" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="2">
-        <v>0.45187878999999997</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0.38677778000000002</v>
-      </c>
-      <c r="H13" s="2"/>
+      <c r="D13" t="s">
+        <v>107</v>
+      </c>
       <c r="I13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="2">
-        <v>0.55299197</v>
-      </c>
-      <c r="L13" s="2">
-        <v>0.36892230576441098</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0.36742376660801201</v>
-      </c>
       <c r="O13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="Q13" s="2">
-        <v>0.77</v>
+        <v>0.45187878999999997</v>
       </c>
       <c r="R13" s="2">
-        <v>0.68</v>
+        <v>0.4</v>
       </c>
       <c r="S13" s="2">
-        <v>0.70378644000000001</v>
+        <v>0.38677778000000002</v>
       </c>
       <c r="T13" s="2"/>
       <c r="U13" s="8" t="s">
         <v>12</v>
       </c>
+      <c r="V13" s="17"/>
+      <c r="W13" s="2">
+        <v>0.55299197</v>
+      </c>
+      <c r="X13" s="2">
+        <v>0.36892230576441098</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>0.36742376660801201</v>
+      </c>
       <c r="AA13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AF13" s="8" t="s">
+      <c r="AC13" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>0.70378644000000001</v>
+      </c>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="AR13" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B14" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>92</v>
+      <c r="D14" t="s">
+        <v>107</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="2">
-        <v>0.53707185999999996</v>
-      </c>
-      <c r="L14" s="2">
-        <v>0.34486215999999997</v>
-      </c>
-      <c r="M14" s="2">
-        <v>0.33676861000000002</v>
-      </c>
       <c r="O14" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="Q14" s="15" t="s">
+        <v>92</v>
+      </c>
       <c r="U14" s="8" t="s">
         <v>13</v>
       </c>
+      <c r="W14" s="2">
+        <v>0.53707185999999996</v>
+      </c>
+      <c r="X14" s="2">
+        <v>0.34486215999999997</v>
+      </c>
+      <c r="Y14" s="2">
+        <v>0.33676861000000002</v>
+      </c>
       <c r="AA14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AF14" s="8" t="s">
+      <c r="AG14" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR14" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="2">
-        <v>0.60946153999999997</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0.47566386999999999</v>
-      </c>
-      <c r="H15" s="2"/>
       <c r="I15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="2">
-        <v>0.61817975999999997</v>
-      </c>
-      <c r="L15" s="2">
-        <v>0.45162907000000002</v>
-      </c>
-      <c r="M15" s="2">
-        <v>0.44334500999999998</v>
-      </c>
       <c r="O15" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="Q15" s="2">
+        <v>0.60946153999999997</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0.47566386999999999</v>
+      </c>
+      <c r="T15" s="2"/>
       <c r="U15" s="8" t="s">
         <v>14</v>
       </c>
+      <c r="V15" s="16"/>
+      <c r="W15" s="2">
+        <v>0.61817975999999997</v>
+      </c>
+      <c r="X15" s="2">
+        <v>0.45162907000000002</v>
+      </c>
+      <c r="Y15" s="2">
+        <v>0.44334500999999998</v>
+      </c>
       <c r="AA15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="AF15" s="8" t="s">
+      <c r="AG15" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:35" x14ac:dyDescent="0.2">
+      <c r="AM15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR15" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="4">
+      <c r="I16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="4">
         <v>0.71651947999999999</v>
       </c>
-      <c r="F16" s="4">
+      <c r="R16" s="4">
         <v>0.6</v>
       </c>
-      <c r="G16" s="4">
+      <c r="S16" s="4">
         <v>0.60289298999999996</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="4">
+      <c r="T16" s="4"/>
+      <c r="U16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="V16" s="16"/>
+      <c r="W16" s="4">
         <v>0.58481218000000001</v>
       </c>
-      <c r="L16" s="4">
+      <c r="X16" s="4">
         <v>0.50075188000000004</v>
       </c>
-      <c r="M16" s="4">
+      <c r="Y16" s="4">
         <v>0.50386770999999997</v>
       </c>
-      <c r="O16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="U16" s="8" t="s">
-        <v>15</v>
-      </c>
       <c r="AA16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AB16">
+      <c r="AG16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AN16">
         <v>0.57588099999999998</v>
       </c>
-      <c r="AC16">
+      <c r="AO16">
         <v>0.49398799999999998</v>
       </c>
-      <c r="AD16">
+      <c r="AP16">
         <v>0.49834000000000001</v>
       </c>
-      <c r="AF16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG16" s="2">
+      <c r="AR16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS16" s="2">
         <v>0.60354452000000003</v>
       </c>
-      <c r="AH16" s="2">
+      <c r="AT16" s="2">
         <v>0.50651955999999998</v>
       </c>
-      <c r="AI16" s="2">
+      <c r="AU16" s="2">
         <v>0.51198105000000005</v>
       </c>
     </row>
-    <row r="17" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E17">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="F17">
-        <v>0.34</v>
-      </c>
-      <c r="G17">
-        <v>0.34663015245623902</v>
-      </c>
       <c r="I17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="2">
-        <v>0.47712673999999999</v>
-      </c>
-      <c r="L17" s="2">
-        <v>0.23208019999999999</v>
-      </c>
-      <c r="M17" s="2">
-        <v>0.17306158999999999</v>
-      </c>
       <c r="O17" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="Q17">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="R17">
+        <v>0.34</v>
+      </c>
+      <c r="S17">
+        <v>0.34663015245623902</v>
+      </c>
       <c r="U17" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="V17" s="17"/>
+      <c r="W17" s="2">
+        <v>0.47712673999999999</v>
+      </c>
+      <c r="X17" s="2">
+        <v>0.23208019999999999</v>
+      </c>
+      <c r="Y17" s="2">
+        <v>0.17306158999999999</v>
+      </c>
       <c r="AA17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="AF17" s="8" t="s">
+      <c r="AG17" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR17" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E18">
-        <v>0.41599999999999998</v>
-      </c>
-      <c r="F18">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="G18">
-        <v>0.30499999999999899</v>
-      </c>
+      <c r="D18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
       <c r="I18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
       <c r="O18" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="Q18">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="R18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="S18">
+        <v>0.30499999999999899</v>
+      </c>
       <c r="U18" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
       <c r="AA18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AF18" s="9" t="s">
+      <c r="AG18" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM18" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AR18" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B19" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E19">
-        <v>0.58186813186813102</v>
-      </c>
-      <c r="F19">
-        <v>0.4</v>
-      </c>
-      <c r="G19">
-        <v>0.39490909090908999</v>
+      <c r="D19" t="s">
+        <v>107</v>
       </c>
       <c r="I19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="2">
-        <v>0.56425099999999995</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0.27619048000000002</v>
-      </c>
-      <c r="M19" s="2">
-        <v>0.24500280999999999</v>
-      </c>
       <c r="O19" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="Q19">
+        <v>0.58186813186813102</v>
+      </c>
+      <c r="R19">
+        <v>0.4</v>
+      </c>
+      <c r="S19">
+        <v>0.39490909090908999</v>
+      </c>
       <c r="U19" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="W19" s="2">
+        <v>0.56425099999999995</v>
+      </c>
+      <c r="X19" s="2">
+        <v>0.27619048000000002</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>0.24500280999999999</v>
+      </c>
       <c r="AA19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="AF19" s="8" t="s">
+      <c r="AG19" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR19" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B20" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="E20">
-        <v>0.50682499999999997</v>
-      </c>
-      <c r="F20">
-        <v>0.36</v>
-      </c>
-      <c r="G20">
-        <v>0.34594900000000001</v>
+      <c r="D20" t="s">
+        <v>107</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
       <c r="O20" s="8" t="s">
         <v>100</v>
       </c>
+      <c r="Q20">
+        <v>0.50682499999999997</v>
+      </c>
+      <c r="R20">
+        <v>0.36</v>
+      </c>
+      <c r="S20">
+        <v>0.34594900000000001</v>
+      </c>
       <c r="U20" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="AA20" s="8"/>
-      <c r="AF20" s="8"/>
-    </row>
-    <row r="21" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="AA20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AG20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AM20" s="8"/>
+      <c r="AR20" s="8"/>
+    </row>
+    <row r="21" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="E21">
-        <v>0.655555555555555</v>
-      </c>
-      <c r="F21">
-        <v>0.38</v>
-      </c>
-      <c r="G21">
-        <v>0.40454545454545399</v>
-      </c>
       <c r="I21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="K21" s="2">
-        <v>0.51212380999999996</v>
-      </c>
-      <c r="L21" s="2">
-        <v>0.27669173000000002</v>
-      </c>
-      <c r="M21" s="2">
-        <v>0.24118174000000001</v>
-      </c>
       <c r="O21" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="Q21">
+        <v>0.655555555555555</v>
+      </c>
+      <c r="R21">
+        <v>0.38</v>
+      </c>
+      <c r="S21">
+        <v>0.40454545454545399</v>
+      </c>
       <c r="U21" s="8" t="s">
         <v>24</v>
       </c>
+      <c r="W21" s="2">
+        <v>0.51212380999999996</v>
+      </c>
+      <c r="X21" s="2">
+        <v>0.27669173000000002</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>0.24118174000000001</v>
+      </c>
       <c r="AA21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AF21" s="8" t="s">
+      <c r="AG21" s="8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM21" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AR21" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B22" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="E22">
-        <v>0.60133333333333305</v>
-      </c>
-      <c r="F22">
-        <v>0.46</v>
-      </c>
-      <c r="G22">
-        <v>0.44543589743589701</v>
-      </c>
       <c r="I22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="K22" s="2">
-        <v>0.49125333999999998</v>
-      </c>
-      <c r="L22" s="2">
-        <v>0.30476189999999997</v>
-      </c>
-      <c r="M22" s="2">
-        <v>0.28231458999999998</v>
-      </c>
       <c r="O22" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="Q22">
+        <v>0.60133333333333305</v>
+      </c>
+      <c r="R22">
+        <v>0.46</v>
+      </c>
+      <c r="S22">
+        <v>0.44543589743589701</v>
+      </c>
       <c r="U22" s="8" t="s">
         <v>25</v>
       </c>
+      <c r="W22" s="2">
+        <v>0.49125333999999998</v>
+      </c>
+      <c r="X22" s="2">
+        <v>0.30476189999999997</v>
+      </c>
+      <c r="Y22" s="2">
+        <v>0.28231458999999998</v>
+      </c>
       <c r="AA22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AF22" s="8" t="s">
+      <c r="AG22" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AR22" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B23" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E23">
-        <v>0.54952380952380897</v>
-      </c>
-      <c r="F23">
-        <v>0.36</v>
-      </c>
-      <c r="G23">
-        <v>0.32374703557312201</v>
+      <c r="D23" t="s">
+        <v>107</v>
       </c>
       <c r="I23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="2">
-        <v>0.48442905000000003</v>
-      </c>
-      <c r="L23" s="2">
-        <v>0.31578947000000002</v>
-      </c>
-      <c r="M23" s="2">
-        <v>0.29657749999999999</v>
-      </c>
       <c r="O23" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="Q23">
+        <v>0.54952380952380897</v>
+      </c>
+      <c r="R23">
+        <v>0.36</v>
+      </c>
+      <c r="S23">
+        <v>0.32374703557312201</v>
+      </c>
       <c r="U23" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="W23" s="2">
+        <v>0.48442905000000003</v>
+      </c>
+      <c r="X23" s="2">
+        <v>0.31578947000000002</v>
+      </c>
+      <c r="Y23" s="2">
+        <v>0.29657749999999999</v>
+      </c>
       <c r="AA23" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AF23" s="8" t="s">
+      <c r="AG23" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AR23" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E24">
-        <v>0.47060606060605997</v>
-      </c>
-      <c r="F24">
-        <v>0.42</v>
-      </c>
-      <c r="G24">
-        <v>0.38861538461538397</v>
+      <c r="D24" t="s">
+        <v>107</v>
       </c>
       <c r="I24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K24" s="2">
-        <v>0.58530731000000003</v>
-      </c>
-      <c r="L24" s="2">
-        <v>0.32130325999999998</v>
-      </c>
-      <c r="M24" s="2">
-        <v>0.31364184000000001</v>
-      </c>
       <c r="O24" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="Q24">
+        <v>0.47060606060605997</v>
+      </c>
+      <c r="R24">
+        <v>0.42</v>
+      </c>
+      <c r="S24">
+        <v>0.38861538461538397</v>
+      </c>
       <c r="U24" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="W24" s="2">
+        <v>0.58530731000000003</v>
+      </c>
+      <c r="X24" s="2">
+        <v>0.32130325999999998</v>
+      </c>
+      <c r="Y24" s="2">
+        <v>0.31364184000000001</v>
+      </c>
       <c r="AA24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AF24" s="8" t="s">
+      <c r="AG24" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM24" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AR24" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="2">
-        <v>0.69446154000000004</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0.52</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0.53914439000000003</v>
-      </c>
-      <c r="H25" s="2"/>
+      <c r="D25" t="s">
+        <v>107</v>
+      </c>
       <c r="I25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J25" s="20"/>
-      <c r="K25">
-        <v>0.60768</v>
-      </c>
-      <c r="L25">
-        <v>0.43959900000000002</v>
-      </c>
-      <c r="M25">
-        <v>0.435585</v>
-      </c>
-      <c r="N25" s="5"/>
       <c r="O25" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="Q25" s="2">
+        <v>0.69446154000000004</v>
+      </c>
+      <c r="R25" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="S25" s="2">
+        <v>0.53914439000000003</v>
+      </c>
+      <c r="T25" s="2"/>
       <c r="U25" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="V25" s="17"/>
+      <c r="W25">
+        <v>0.60768</v>
+      </c>
+      <c r="X25">
+        <v>0.43959900000000002</v>
+      </c>
+      <c r="Y25">
+        <v>0.435585</v>
+      </c>
+      <c r="Z25" s="5"/>
       <c r="AA25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AF25" s="8" t="s">
+      <c r="AG25" s="8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR25" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="2">
-        <v>0.57015583999999997</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0.54</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0.51797541999999996</v>
-      </c>
-      <c r="H26" s="2"/>
+      <c r="D26" t="s">
+        <v>107</v>
+      </c>
       <c r="I26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="J26" s="20"/>
-      <c r="K26" s="2">
-        <v>0.58421833999999995</v>
-      </c>
-      <c r="L26" s="2">
-        <v>0.47518797000000002</v>
-      </c>
-      <c r="M26" s="2">
-        <v>0.48158585999999998</v>
-      </c>
       <c r="O26" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="Q26" s="2">
+        <v>0.57015583999999997</v>
+      </c>
+      <c r="R26" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="S26" s="2">
+        <v>0.51797541999999996</v>
+      </c>
+      <c r="T26" s="2"/>
       <c r="U26" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="V26" s="17"/>
+      <c r="W26" s="2">
+        <v>0.58421833999999995</v>
+      </c>
+      <c r="X26" s="2">
+        <v>0.47518797000000002</v>
+      </c>
+      <c r="Y26" s="2">
+        <v>0.48158585999999998</v>
+      </c>
       <c r="AA26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AF26" s="8" t="s">
+      <c r="AG26" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM26" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AR26" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B27" s="8" t="s">
         <v>91</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E27">
-        <v>0.52248499999999998</v>
-      </c>
-      <c r="F27">
-        <v>0.46</v>
-      </c>
-      <c r="G27">
-        <v>0.44462800000000002</v>
+      <c r="D27" t="s">
+        <v>107</v>
       </c>
       <c r="I27" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="K27">
-        <v>0.54705800000000004</v>
-      </c>
-      <c r="L27">
-        <v>0.34536299999999998</v>
-      </c>
-      <c r="M27">
-        <v>0.33741700000000002</v>
-      </c>
       <c r="O27" s="8" t="s">
         <v>91</v>
       </c>
+      <c r="Q27">
+        <v>0.52248499999999998</v>
+      </c>
+      <c r="R27">
+        <v>0.46</v>
+      </c>
+      <c r="S27">
+        <v>0.44462800000000002</v>
+      </c>
       <c r="U27" s="8" t="s">
         <v>91</v>
       </c>
+      <c r="W27">
+        <v>0.54705800000000004</v>
+      </c>
+      <c r="X27">
+        <v>0.34536299999999998</v>
+      </c>
+      <c r="Y27">
+        <v>0.33741700000000002</v>
+      </c>
       <c r="AA27" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="AF27" s="8" t="s">
+      <c r="AG27" s="8" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="28" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM27" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR27" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
         <v>99</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E28">
-        <v>0.61444399999999999</v>
-      </c>
-      <c r="F28">
-        <v>0.4</v>
-      </c>
-      <c r="G28">
-        <v>0.38377099999999997</v>
-      </c>
       <c r="I28" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="K28">
-        <v>0.564828</v>
-      </c>
-      <c r="L28">
-        <v>0.27468700000000001</v>
-      </c>
-      <c r="M28">
-        <v>0.24404999999999999</v>
-      </c>
       <c r="O28" s="8" t="s">
         <v>99</v>
       </c>
+      <c r="Q28">
+        <v>0.61444399999999999</v>
+      </c>
+      <c r="R28">
+        <v>0.4</v>
+      </c>
+      <c r="S28">
+        <v>0.38377099999999997</v>
+      </c>
       <c r="U28" s="8" t="s">
         <v>99</v>
       </c>
+      <c r="W28">
+        <v>0.564828</v>
+      </c>
+      <c r="X28">
+        <v>0.27468700000000001</v>
+      </c>
+      <c r="Y28">
+        <v>0.24404999999999999</v>
+      </c>
       <c r="AA28" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AF28" s="8" t="s">
+      <c r="AG28" s="8" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="30" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="AM28" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AR28" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="2:44" x14ac:dyDescent="0.2">
       <c r="C30" s="14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:44" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="AG2:AI2"/>
+  <mergeCells count="8">
+    <mergeCell ref="AN2:AP2"/>
+    <mergeCell ref="AS2:AU2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="K2:M2"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="Q2:S2"/>
-    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="Q2:T2"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4097,8 +4390,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4172,20 +4465,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="G1" s="18" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="G1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -4788,20 +5081,20 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="G43" s="18" t="s">
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="G43" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">

</xml_diff>

<commit_message>
finished test-experiments on gpt-3.5, started specific experiments on gpt-4
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts.xlsx
+++ b/models/evaluations/evaluation_prompts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8CE6A4-2525-E448-928B-F1E147D2BE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E064E5D9-B7CA-B146-8C49-6842EEEA357D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -944,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
-  <dimension ref="B2:AU32"/>
+  <dimension ref="B2:AU43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:G8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1140,6 +1140,16 @@
       <c r="I4" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="J4" s="17"/>
+      <c r="K4">
+        <v>0.58704400000000001</v>
+      </c>
+      <c r="L4">
+        <v>0.41336600000000001</v>
+      </c>
+      <c r="M4">
+        <v>0.39852399999999999</v>
+      </c>
       <c r="O4" s="8" t="s">
         <v>5</v>
       </c>
@@ -1435,6 +1445,15 @@
       <c r="D9" t="s">
         <v>107</v>
       </c>
+      <c r="E9">
+        <v>0.48905399999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.31188100000000002</v>
+      </c>
+      <c r="G9">
+        <v>0.29295399999999999</v>
+      </c>
       <c r="I9" s="8" t="s">
         <v>9</v>
       </c>
@@ -1496,6 +1515,15 @@
       <c r="D10" t="s">
         <v>107</v>
       </c>
+      <c r="E10">
+        <v>0.54530100000000004</v>
+      </c>
+      <c r="F10">
+        <v>0.29455399999999998</v>
+      </c>
+      <c r="G10">
+        <v>0.269202</v>
+      </c>
       <c r="I10" s="8" t="s">
         <v>10</v>
       </c>
@@ -1556,6 +1584,15 @@
       </c>
       <c r="D11" t="s">
         <v>107</v>
+      </c>
+      <c r="E11">
+        <v>0.497809</v>
+      </c>
+      <c r="F11">
+        <v>0.316832</v>
+      </c>
+      <c r="G11">
+        <v>0.297539</v>
       </c>
       <c r="I11" s="8" t="s">
         <v>21</v>
@@ -1655,8 +1692,27 @@
       <c r="D13" t="s">
         <v>107</v>
       </c>
+      <c r="E13">
+        <v>0.54598999999999998</v>
+      </c>
+      <c r="F13">
+        <v>0.35396</v>
+      </c>
+      <c r="G13">
+        <v>0.34911799999999998</v>
+      </c>
       <c r="I13" s="8" t="s">
         <v>12</v>
+      </c>
+      <c r="J13" s="17"/>
+      <c r="K13">
+        <v>0.69281700000000002</v>
+      </c>
+      <c r="L13">
+        <v>0.53712899999999997</v>
+      </c>
+      <c r="M13">
+        <v>0.556975</v>
       </c>
       <c r="O13" s="8" t="s">
         <v>12</v>
@@ -1717,6 +1773,15 @@
       <c r="D14" t="s">
         <v>107</v>
       </c>
+      <c r="E14">
+        <v>0.43309799999999998</v>
+      </c>
+      <c r="F14">
+        <v>0.341584</v>
+      </c>
+      <c r="G14">
+        <v>0.319803</v>
+      </c>
       <c r="I14" s="8" t="s">
         <v>13</v>
       </c>
@@ -1758,8 +1823,27 @@
       <c r="C15" s="11" t="s">
         <v>42</v>
       </c>
+      <c r="E15">
+        <v>0.60474300000000003</v>
+      </c>
+      <c r="F15">
+        <v>0.41831699999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.41343099999999999</v>
+      </c>
       <c r="I15" s="8" t="s">
         <v>14</v>
+      </c>
+      <c r="J15" s="16"/>
+      <c r="K15">
+        <v>0.691137</v>
+      </c>
+      <c r="L15">
+        <v>0.53217800000000004</v>
+      </c>
+      <c r="M15">
+        <v>0.55549099999999996</v>
       </c>
       <c r="O15" s="8" t="s">
         <v>14</v>
@@ -1807,9 +1891,19 @@
       <c r="C16" s="11" t="s">
         <v>46</v>
       </c>
+      <c r="E16">
+        <v>0.55871099999999996</v>
+      </c>
+      <c r="F16">
+        <v>0.485149</v>
+      </c>
+      <c r="G16">
+        <v>0.47761999999999999</v>
+      </c>
       <c r="I16" s="8" t="s">
         <v>15</v>
       </c>
+      <c r="J16" s="16"/>
       <c r="O16" s="8" t="s">
         <v>15</v>
       </c>
@@ -1874,9 +1968,19 @@
       <c r="C17" s="11" t="s">
         <v>58</v>
       </c>
+      <c r="E17">
+        <v>0.60226999999999997</v>
+      </c>
+      <c r="F17">
+        <v>0.235149</v>
+      </c>
+      <c r="G17">
+        <v>0.191112</v>
+      </c>
       <c r="I17" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="J17" s="17"/>
       <c r="O17" s="8" t="s">
         <v>16</v>
       </c>
@@ -1972,6 +2076,15 @@
       <c r="D19" t="s">
         <v>107</v>
       </c>
+      <c r="E19">
+        <v>0.43840600000000002</v>
+      </c>
+      <c r="F19">
+        <v>0.27722799999999997</v>
+      </c>
+      <c r="G19">
+        <v>0.237849</v>
+      </c>
       <c r="I19" s="8" t="s">
         <v>18</v>
       </c>
@@ -2021,6 +2134,15 @@
       </c>
       <c r="D20" t="s">
         <v>107</v>
+      </c>
+      <c r="E20">
+        <v>0.52865600000000001</v>
+      </c>
+      <c r="F20">
+        <v>0.28960399999999997</v>
+      </c>
+      <c r="G20">
+        <v>0.26192700000000002</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>100</v>
@@ -2059,6 +2181,15 @@
       <c r="C21" s="11" t="s">
         <v>33</v>
       </c>
+      <c r="E21">
+        <v>0.47489900000000002</v>
+      </c>
+      <c r="F21">
+        <v>0.28712900000000002</v>
+      </c>
+      <c r="G21">
+        <v>0.25231799999999999</v>
+      </c>
       <c r="I21" s="8" t="s">
         <v>24</v>
       </c>
@@ -2106,6 +2237,15 @@
       <c r="C22" s="11" t="s">
         <v>94</v>
       </c>
+      <c r="E22">
+        <v>0.499913</v>
+      </c>
+      <c r="F22">
+        <v>0.329208</v>
+      </c>
+      <c r="G22">
+        <v>0.30395699999999998</v>
+      </c>
       <c r="I22" s="8" t="s">
         <v>25</v>
       </c>
@@ -2156,6 +2296,15 @@
       <c r="D23" t="s">
         <v>107</v>
       </c>
+      <c r="E23">
+        <v>0.46459899999999998</v>
+      </c>
+      <c r="F23">
+        <v>0.30940600000000001</v>
+      </c>
+      <c r="G23">
+        <v>0.28628999999999999</v>
+      </c>
       <c r="I23" s="8" t="s">
         <v>26</v>
       </c>
@@ -2206,6 +2355,15 @@
       <c r="D24" t="s">
         <v>107</v>
       </c>
+      <c r="E24">
+        <v>0.48017300000000002</v>
+      </c>
+      <c r="F24">
+        <v>0.30198000000000003</v>
+      </c>
+      <c r="G24">
+        <v>0.27839900000000001</v>
+      </c>
       <c r="I24" s="8" t="s">
         <v>27</v>
       </c>
@@ -2256,9 +2414,19 @@
       <c r="D25" t="s">
         <v>107</v>
       </c>
+      <c r="E25">
+        <v>0.60309599999999997</v>
+      </c>
+      <c r="F25">
+        <v>0.41831699999999999</v>
+      </c>
+      <c r="G25">
+        <v>0.41634399999999999</v>
+      </c>
       <c r="I25" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="J25" s="17"/>
       <c r="O25" s="8" t="s">
         <v>28</v>
       </c>
@@ -2309,9 +2477,19 @@
       <c r="D26" t="s">
         <v>107</v>
       </c>
+      <c r="E26">
+        <v>0.53626799999999997</v>
+      </c>
+      <c r="F26">
+        <v>0.43069299999999999</v>
+      </c>
+      <c r="G26">
+        <v>0.42550700000000002</v>
+      </c>
       <c r="I26" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="J26" s="17"/>
       <c r="O26" s="8" t="s">
         <v>29</v>
       </c>
@@ -2361,6 +2539,15 @@
       <c r="D27" t="s">
         <v>107</v>
       </c>
+      <c r="E27">
+        <v>0.61195900000000003</v>
+      </c>
+      <c r="F27">
+        <v>0.35643599999999998</v>
+      </c>
+      <c r="G27">
+        <v>0.34517799999999998</v>
+      </c>
       <c r="I27" s="8" t="s">
         <v>91</v>
       </c>
@@ -2408,6 +2595,15 @@
       <c r="C28" s="11" t="s">
         <v>102</v>
       </c>
+      <c r="E28">
+        <v>0.55375399999999997</v>
+      </c>
+      <c r="F28">
+        <v>0.27722799999999997</v>
+      </c>
+      <c r="G28">
+        <v>0.24971199999999999</v>
+      </c>
       <c r="I28" s="8" t="s">
         <v>99</v>
       </c>
@@ -2457,6 +2653,12 @@
       <c r="B32" t="s">
         <v>104</v>
       </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="13"/>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
P6, P7, P11_3, P11_4, i.e. finished testss on gpt-4 except for binary classification and ICL
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts.xlsx
+++ b/models/evaluations/evaluation_prompts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E064E5D9-B7CA-B146-8C49-6842EEEA357D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1F54F5-9D63-184C-86E1-511340591701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="109">
   <si>
     <t>prompt description</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>4_1 gpt 4 test vs gpt4 test 50: in grand scheme comparable, not all classes depicted or not in same way</t>
   </si>
 </sst>
 </file>
@@ -946,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
   <dimension ref="B2:AU43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1904,6 +1907,15 @@
         <v>15</v>
       </c>
       <c r="J16" s="16"/>
+      <c r="K16" s="14">
+        <v>0.70457400000000003</v>
+      </c>
+      <c r="L16" s="14">
+        <v>0.53712899999999997</v>
+      </c>
+      <c r="M16" s="14">
+        <v>0.57348399999999999</v>
+      </c>
       <c r="O16" s="8" t="s">
         <v>15</v>
       </c>
@@ -1981,6 +1993,15 @@
         <v>16</v>
       </c>
       <c r="J17" s="17"/>
+      <c r="K17">
+        <v>0.58668799999999999</v>
+      </c>
+      <c r="L17">
+        <v>0.38861400000000001</v>
+      </c>
+      <c r="M17">
+        <v>0.34958600000000001</v>
+      </c>
       <c r="O17" s="8" t="s">
         <v>16</v>
       </c>
@@ -2427,6 +2448,15 @@
         <v>28</v>
       </c>
       <c r="J25" s="17"/>
+      <c r="K25">
+        <v>0.69020999999999999</v>
+      </c>
+      <c r="L25">
+        <v>0.54455399999999998</v>
+      </c>
+      <c r="M25">
+        <v>0.560608</v>
+      </c>
       <c r="O25" s="8" t="s">
         <v>28</v>
       </c>
@@ -2490,6 +2520,15 @@
         <v>29</v>
       </c>
       <c r="J26" s="17"/>
+      <c r="K26">
+        <v>0.69849899999999998</v>
+      </c>
+      <c r="L26">
+        <v>0.54207899999999998</v>
+      </c>
+      <c r="M26">
+        <v>0.57139099999999998</v>
+      </c>
       <c r="O26" s="8" t="s">
         <v>29</v>
       </c>
@@ -2647,6 +2686,11 @@
     <row r="30" spans="2:44" x14ac:dyDescent="0.2">
       <c r="C30" s="14" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="2:44" x14ac:dyDescent="0.2">
+      <c r="K31" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="2:44" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
tried stepbystep-labelin (not succeeded yet) and proved that P9_1 does give explanation
</commit_message>
<xml_diff>
--- a/models/evaluations/evaluation_prompts.xlsx
+++ b/models/evaluations/evaluation_prompts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shirin 1/git/PreclinicalAbstractClassification/models/evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1F54F5-9D63-184C-86E1-511340591701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADCBE91-BACA-6144-AEAD-9FFAF3A13837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{8DEB04AB-2159-B140-83EF-22DC4E795892}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="111">
   <si>
     <t>prompt description</t>
   </si>
@@ -420,12 +420,6 @@
     <t>2CoT&amp;CC: P11 &amp; explanation (CoT) based on P9</t>
   </si>
   <si>
-    <t>does P9/P9_1/P12 really give explanation??</t>
-  </si>
-  <si>
-    <t>description of P11- P11_2 was wrong (only table!); P9_1 new, P11_5 and P12 new; first half and then second half P6 new</t>
-  </si>
-  <si>
     <t>summary 0.2test gpt-3.5</t>
   </si>
   <si>
@@ -436,6 +430,18 @@
   </si>
   <si>
     <t>4_1 gpt 4 test vs gpt4 test 50: in grand scheme comparable, not all classes depicted or not in same way</t>
+  </si>
+  <si>
+    <t>gpt-4 deutlich besser</t>
+  </si>
+  <si>
+    <t>P6 am besten</t>
+  </si>
+  <si>
+    <t>P8: step-by-step-labeling mit step-by-step code umsetzen? (Hilfe)</t>
+  </si>
+  <si>
+    <t>wenn ich neue Prompts entwickle, muss icha fu train machen und dann auf test laufen lassen, damit kein Overfitting</t>
   </si>
 </sst>
 </file>
@@ -580,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -608,6 +614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E17E8F-075F-B54C-ACF4-C049684AF8E3}">
   <dimension ref="B2:AU43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="85" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -976,12 +983,12 @@
   <sheetData>
     <row r="2" spans="2:47" x14ac:dyDescent="0.2">
       <c r="E2" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="18"/>
       <c r="K2" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L2" s="18"/>
       <c r="M2" s="18"/>
@@ -1281,7 +1288,7 @@
         <v>62</v>
       </c>
       <c r="D6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -1329,7 +1336,7 @@
         <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -1376,7 +1383,7 @@
         <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E8">
         <v>0.59226599999999996</v>
@@ -1446,7 +1453,7 @@
         <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E9">
         <v>0.48905399999999999</v>
@@ -1516,7 +1523,7 @@
         <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E10">
         <v>0.54530100000000004</v>
@@ -1586,7 +1593,7 @@
         <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E11">
         <v>0.497809</v>
@@ -1646,7 +1653,7 @@
         <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -1693,7 +1700,7 @@
         <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13">
         <v>0.54598999999999998</v>
@@ -1774,7 +1781,7 @@
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E14">
         <v>0.43309799999999998</v>
@@ -2048,7 +2055,7 @@
         <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
@@ -2095,7 +2102,7 @@
         <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E19">
         <v>0.43840600000000002</v>
@@ -2154,7 +2161,7 @@
         <v>101</v>
       </c>
       <c r="D20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E20">
         <v>0.52865600000000001</v>
@@ -2315,7 +2322,7 @@
         <v>95</v>
       </c>
       <c r="D23" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E23">
         <v>0.46459899999999998</v>
@@ -2374,7 +2381,7 @@
         <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E24">
         <v>0.48017300000000002</v>
@@ -2433,7 +2440,7 @@
         <v>34</v>
       </c>
       <c r="D25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E25">
         <v>0.60309599999999997</v>
@@ -2505,7 +2512,7 @@
         <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E26">
         <v>0.53626799999999997</v>
@@ -2576,7 +2583,7 @@
         <v>93</v>
       </c>
       <c r="D27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E27">
         <v>0.61195900000000003</v>
@@ -2684,24 +2691,37 @@
       </c>
     </row>
     <row r="30" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="C30" s="14" t="s">
-        <v>103</v>
-      </c>
+      <c r="C30" s="21"/>
     </row>
     <row r="31" spans="2:44" x14ac:dyDescent="0.2">
       <c r="K31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="K33" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="K34" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="32" spans="2:44" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="K35" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="K36" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C42" s="13"/>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C43" s="13"/>
     </row>
   </sheetData>

</xml_diff>